<commit_message>
[TEX] Kupferpaneel; Sprachdatei de geupdated
</commit_message>
<xml_diff>
--- a/Versandordner/Assets (technisch)/Sprachdateilisten.xlsx
+++ b/Versandordner/Assets (technisch)/Sprachdateilisten.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\Documents\GitHub\MCMOD-RedTec\Versandordner\Assets (technisch)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frieb\Documents\GitHub\MCMOD-Industria\Versandordner\Assets (technisch)\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="118">
   <si>
     <t>monel_dust</t>
   </si>
@@ -216,12 +216,174 @@
   </si>
   <si>
     <t>YKNIL AKŽĹD</t>
+  </si>
+  <si>
+    <t>exposed_iron_block</t>
+  </si>
+  <si>
+    <t>weathered_iron_block</t>
+  </si>
+  <si>
+    <t>oxidized_iron_block</t>
+  </si>
+  <si>
+    <t>exposed_iron_plates</t>
+  </si>
+  <si>
+    <t>weathered_iron_plates</t>
+  </si>
+  <si>
+    <t>oxidized_iron_plates</t>
+  </si>
+  <si>
+    <t>waxed_exposed_iron_block</t>
+  </si>
+  <si>
+    <t>waxed_weathered_iron_block</t>
+  </si>
+  <si>
+    <t>waxed_oxidized_iron_block</t>
+  </si>
+  <si>
+    <t>waxed_exposed_iron_plates</t>
+  </si>
+  <si>
+    <t>waxed_weathered_iron_plates</t>
+  </si>
+  <si>
+    <t>waxed_oxidized_iron_plates</t>
+  </si>
+  <si>
+    <t>exposed_copper_plates</t>
+  </si>
+  <si>
+    <t>weathered_copper_plates</t>
+  </si>
+  <si>
+    <t>oxidized_copper_plates</t>
+  </si>
+  <si>
+    <t>waxed_exposed_copper_plates</t>
+  </si>
+  <si>
+    <t>waxed_weathered_copper_plates</t>
+  </si>
+  <si>
+    <t>waxed_oxidized_copper_plates</t>
+  </si>
+  <si>
+    <t>exposed_steel_block</t>
+  </si>
+  <si>
+    <t>weathered_steel_block</t>
+  </si>
+  <si>
+    <t>oxidized_steel_block</t>
+  </si>
+  <si>
+    <t>exposed_steel_plates</t>
+  </si>
+  <si>
+    <t>weathered_steel_plates</t>
+  </si>
+  <si>
+    <t>oxidized_steel_plates</t>
+  </si>
+  <si>
+    <t>waxed_exposed_steel_block</t>
+  </si>
+  <si>
+    <t>waxed_weathered_steel_block</t>
+  </si>
+  <si>
+    <t>waxed_oxidized_steel_block</t>
+  </si>
+  <si>
+    <t>waxed_exposed_steel_plates</t>
+  </si>
+  <si>
+    <t>waxed_weathered_steel_plates</t>
+  </si>
+  <si>
+    <t>waxed_oxidized_steel_plates</t>
+  </si>
+  <si>
+    <t>exposed_tin_block</t>
+  </si>
+  <si>
+    <t>weathered_tin_block</t>
+  </si>
+  <si>
+    <t>oxidized_tin_block</t>
+  </si>
+  <si>
+    <t>exposed_tin_plates</t>
+  </si>
+  <si>
+    <t>weathered_tin_plates</t>
+  </si>
+  <si>
+    <t>oxidized_tin_plates</t>
+  </si>
+  <si>
+    <t>waxed_exposed_tin_block</t>
+  </si>
+  <si>
+    <t>waxed_weathered_tin_block</t>
+  </si>
+  <si>
+    <t>waxed_oxidized_tin_block</t>
+  </si>
+  <si>
+    <t>waxed_exposed_tin_plates</t>
+  </si>
+  <si>
+    <t>waxed_weathered_tin_plates</t>
+  </si>
+  <si>
+    <t>waxed_oxidized_tin_plates</t>
+  </si>
+  <si>
+    <t>exposed_brass_block</t>
+  </si>
+  <si>
+    <t>weathered_brass_block</t>
+  </si>
+  <si>
+    <t>oxidized_brass_block</t>
+  </si>
+  <si>
+    <t>exposed_brass_plates</t>
+  </si>
+  <si>
+    <t>weathered_brass_plates</t>
+  </si>
+  <si>
+    <t>oxidized_brass_plates</t>
+  </si>
+  <si>
+    <t>waxed_exposed_brass_block</t>
+  </si>
+  <si>
+    <t>waxed_weathered_brass_block</t>
+  </si>
+  <si>
+    <t>waxed_oxidized_brass_block</t>
+  </si>
+  <si>
+    <t>waxed_exposed_brass_plates</t>
+  </si>
+  <si>
+    <t>waxed_weathered_brass_plates</t>
+  </si>
+  <si>
+    <t>waxed_oxidized_brass_plates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -301,7 +463,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -566,12 +728,12 @@
   <dimension ref="A2:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -581,8 +743,17 @@
       <c r="C2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -592,8 +763,17 @@
       <c r="C3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -603,8 +783,17 @@
       <c r="C4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -614,8 +803,17 @@
       <c r="C5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -625,8 +823,17 @@
       <c r="C6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -636,8 +843,17 @@
       <c r="C7" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -647,8 +863,17 @@
       <c r="C8" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -658,8 +883,17 @@
       <c r="C9" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -669,8 +903,17 @@
       <c r="C10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -680,8 +923,17 @@
       <c r="C11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -691,8 +943,17 @@
       <c r="C12" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -702,8 +963,17 @@
       <c r="C13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -713,8 +983,17 @@
       <c r="C14" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -724,8 +1003,17 @@
       <c r="C15" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -735,6 +1023,15 @@
       <c r="C16" t="s">
         <v>61</v>
       </c>
+      <c r="E16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -746,6 +1043,15 @@
       <c r="C17" t="s">
         <v>61</v>
       </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -757,6 +1063,15 @@
       <c r="C18" t="s">
         <v>61</v>
       </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -768,6 +1083,15 @@
       <c r="C19" t="s">
         <v>61</v>
       </c>
+      <c r="E19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -779,6 +1103,15 @@
       <c r="C20" t="s">
         <v>61</v>
       </c>
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -790,6 +1123,15 @@
       <c r="C21" t="s">
         <v>61</v>
       </c>
+      <c r="E21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -801,6 +1143,15 @@
       <c r="C22" t="s">
         <v>61</v>
       </c>
+      <c r="E22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -812,6 +1163,15 @@
       <c r="C23" t="s">
         <v>61</v>
       </c>
+      <c r="E23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -823,6 +1183,15 @@
       <c r="C24" t="s">
         <v>61</v>
       </c>
+      <c r="E24" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -834,6 +1203,15 @@
       <c r="C25" t="s">
         <v>61</v>
       </c>
+      <c r="E25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -845,6 +1223,15 @@
       <c r="C26" t="s">
         <v>61</v>
       </c>
+      <c r="E26" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -856,6 +1243,15 @@
       <c r="C27" t="s">
         <v>61</v>
       </c>
+      <c r="E27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -867,6 +1263,15 @@
       <c r="C28" t="s">
         <v>61</v>
       </c>
+      <c r="E28" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -878,6 +1283,15 @@
       <c r="C29" t="s">
         <v>61</v>
       </c>
+      <c r="E29" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G29" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -889,6 +1303,15 @@
       <c r="C30" t="s">
         <v>61</v>
       </c>
+      <c r="E30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" t="s">
+        <v>92</v>
+      </c>
+      <c r="G30" t="s">
+        <v>61</v>
+      </c>
       <c r="N30" s="1" t="s">
         <v>62</v>
       </c>
@@ -903,6 +1326,15 @@
       <c r="C31" t="s">
         <v>61</v>
       </c>
+      <c r="E31" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" t="s">
+        <v>93</v>
+      </c>
+      <c r="G31" t="s">
+        <v>61</v>
+      </c>
       <c r="N31" s="2" t="s">
         <v>63</v>
       </c>
@@ -917,8 +1349,17 @@
       <c r="C32" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" t="s">
+        <v>94</v>
+      </c>
+      <c r="G32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -928,8 +1369,17 @@
       <c r="C33" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -939,8 +1389,17 @@
       <c r="C34" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" t="s">
+        <v>96</v>
+      </c>
+      <c r="G34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -950,8 +1409,17 @@
       <c r="C35" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" t="s">
+        <v>97</v>
+      </c>
+      <c r="G35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -961,8 +1429,17 @@
       <c r="C36" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>60</v>
+      </c>
+      <c r="F36" t="s">
+        <v>98</v>
+      </c>
+      <c r="G36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -972,8 +1449,17 @@
       <c r="C37" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>60</v>
       </c>
@@ -983,8 +1469,17 @@
       <c r="C38" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>60</v>
+      </c>
+      <c r="F38" t="s">
+        <v>100</v>
+      </c>
+      <c r="G38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -994,8 +1489,17 @@
       <c r="C39" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" t="s">
+        <v>101</v>
+      </c>
+      <c r="G39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>60</v>
       </c>
@@ -1005,8 +1509,17 @@
       <c r="C40" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>60</v>
+      </c>
+      <c r="F40" t="s">
+        <v>102</v>
+      </c>
+      <c r="G40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>60</v>
       </c>
@@ -1016,8 +1529,17 @@
       <c r="C41" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" t="s">
+        <v>103</v>
+      </c>
+      <c r="G41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>60</v>
       </c>
@@ -1027,8 +1549,17 @@
       <c r="C42" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" t="s">
+        <v>104</v>
+      </c>
+      <c r="G42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -1038,8 +1569,17 @@
       <c r="C43" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>60</v>
+      </c>
+      <c r="F43" t="s">
+        <v>105</v>
+      </c>
+      <c r="G43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -1049,8 +1589,17 @@
       <c r="C44" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>60</v>
+      </c>
+      <c r="F44" t="s">
+        <v>106</v>
+      </c>
+      <c r="G44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -1060,8 +1609,17 @@
       <c r="C45" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" t="s">
+        <v>107</v>
+      </c>
+      <c r="G45" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -1071,8 +1629,17 @@
       <c r="C46" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>60</v>
+      </c>
+      <c r="F46" t="s">
+        <v>108</v>
+      </c>
+      <c r="G46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -1082,8 +1649,17 @@
       <c r="C47" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>60</v>
+      </c>
+      <c r="F47" t="s">
+        <v>109</v>
+      </c>
+      <c r="G47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -1093,8 +1669,17 @@
       <c r="C48" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48" t="s">
+        <v>110</v>
+      </c>
+      <c r="G48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -1104,8 +1689,17 @@
       <c r="C49" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>60</v>
+      </c>
+      <c r="F49" t="s">
+        <v>111</v>
+      </c>
+      <c r="G49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -1115,8 +1709,17 @@
       <c r="C50" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>60</v>
+      </c>
+      <c r="F50" t="s">
+        <v>112</v>
+      </c>
+      <c r="G50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -1126,8 +1729,17 @@
       <c r="C51" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>60</v>
+      </c>
+      <c r="F51" t="s">
+        <v>113</v>
+      </c>
+      <c r="G51" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -1137,8 +1749,17 @@
       <c r="C52" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>60</v>
+      </c>
+      <c r="F52" t="s">
+        <v>114</v>
+      </c>
+      <c r="G52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -1148,8 +1769,17 @@
       <c r="C53" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>60</v>
+      </c>
+      <c r="F53" t="s">
+        <v>115</v>
+      </c>
+      <c r="G53" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -1159,8 +1789,17 @@
       <c r="C54" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>60</v>
+      </c>
+      <c r="F54" t="s">
+        <v>116</v>
+      </c>
+      <c r="G54" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -1170,8 +1809,17 @@
       <c r="C55" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>60</v>
+      </c>
+      <c r="F55" t="s">
+        <v>117</v>
+      </c>
+      <c r="G55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -1182,7 +1830,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -1193,7 +1841,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -1204,7 +1852,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -1215,7 +1863,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -1226,7 +1874,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>

</xml_diff>